<commit_message>
Expanded functionality of EnergySource
-can now set industry variables - interest, loan period, co2 tax, and land tax
-added methods to handle industry variables
-updated CSV files
-cleaned up data_csv.py
</commit_message>
<xml_diff>
--- a/source_data.xlsx
+++ b/source_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poohb\Desktop\School\Fall_2021\Personal Programming\Demand_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFCF1DB-D6F4-46A7-8FBC-07C8800E0003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A536AC12-7698-42D1-A304-FCF0C318C920}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="14964" windowHeight="10056" xr2:uid="{83F0E00F-F691-4BB6-90EA-7715B153EC09}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83F0E00F-F691-4BB6-90EA-7715B153EC09}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="source_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Onshore Wind</t>
+  </si>
+  <si>
+    <t>Rooftop Solar PV</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,6 +594,12 @@
       <c r="J2">
         <v>0.47499999999999998</v>
       </c>
+      <c r="K2">
+        <v>96</v>
+      </c>
+      <c r="M2">
+        <v>8000</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -617,6 +626,12 @@
       <c r="J3">
         <v>0.56799999999999995</v>
       </c>
+      <c r="K3">
+        <v>57</v>
+      </c>
+      <c r="M3">
+        <v>2000</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -632,7 +647,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G4">
-        <v>114.3</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>10450</v>
@@ -642,6 +657,9 @@
       </c>
       <c r="J4">
         <v>0.93500000000000005</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -660,8 +678,14 @@
       <c r="J5">
         <v>0.34799999999999998</v>
       </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6">
         <v>2671</v>
       </c>
@@ -673,6 +697,9 @@
       </c>
       <c r="J6">
         <v>0.245</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>